<commit_message>
command line tool to send jtl to sql directly
</commit_message>
<xml_diff>
--- a/jmeter/floodios2f.xlsx
+++ b/jmeter/floodios2f.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\PublicTestProjects\jmeter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{54878295-7F27-497C-AD9D-6DFEA21AB5A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{569ED0C8-1745-4A31-A415-4106CEBF0212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120"/>
   </bookViews>
@@ -686,13 +686,13 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -738,12 +738,39 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="11">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -763,10 +790,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.4</cx:f>
       </cx:strDim>
       <cx:numDim type="size">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -804,7 +831,7 @@
         <cx:series layoutId="treemap" uniqueId="{87D1A352-CFAE-4E7F-8877-41635CA904B1}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:f>_xlchart.v1.5</cx:f>
               <cx:v>impact</cx:v>
             </cx:txData>
           </cx:tx>
@@ -827,10 +854,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.4</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.9</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -868,7 +895,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{E0A88D00-FFBD-40CE-8674-020402C000B4}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.5</cx:f>
+              <cx:f>_xlchart.v1.8</cx:f>
               <cx:v>impact</cx:v>
             </cx:txData>
           </cx:tx>
@@ -2015,16 +2042,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>123824</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>193097</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>43296</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>535999</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>109971</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -2060,8 +2087,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5095874" y="857250"/>
-              <a:ext cx="9515476" cy="8458200"/>
+              <a:off x="6375688" y="614796"/>
+              <a:ext cx="9434947" cy="8448675"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2093,16 +2120,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>333374</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>51089</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>42429</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>171449</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>467592</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>17318</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -2138,8 +2165,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="15059024" y="1943100"/>
-              <a:ext cx="8372475" cy="5867400"/>
+              <a:off x="5021407" y="9567429"/>
+              <a:ext cx="12539230" cy="6832889"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2936,21 +2963,24 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L35" totalsRowShown="0">
   <autoFilter ref="A1:L35"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L35">
+    <sortCondition descending="1" ref="B1:B35"/>
+  </sortState>
   <tableColumns count="12">
     <tableColumn id="1" name="Label"/>
-    <tableColumn id="2" name="# Samples"/>
-    <tableColumn id="3" name="Average"/>
-    <tableColumn id="4" name="Min"/>
-    <tableColumn id="5" name="Max"/>
-    <tableColumn id="6" name="Std. Dev."/>
-    <tableColumn id="7" name="Error %" dataDxfId="1"/>
-    <tableColumn id="8" name="Throughput"/>
-    <tableColumn id="9" name="Received KB/sec"/>
-    <tableColumn id="10" name="Sent KB/sec"/>
-    <tableColumn id="11" name="Avg. Bytes"/>
-    <tableColumn id="12" name="Impact" dataDxfId="0">
+    <tableColumn id="12" name="Impact" dataDxfId="10">
       <calculatedColumnFormula>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="2" name="# Samples" dataDxfId="9"/>
+    <tableColumn id="3" name="Average" dataDxfId="8"/>
+    <tableColumn id="4" name="Min" dataDxfId="7"/>
+    <tableColumn id="5" name="Max" dataDxfId="6"/>
+    <tableColumn id="6" name="Std. Dev." dataDxfId="5"/>
+    <tableColumn id="7" name="Error %" dataDxfId="4"/>
+    <tableColumn id="8" name="Throughput" dataDxfId="3"/>
+    <tableColumn id="9" name="Received KB/sec" dataDxfId="2"/>
+    <tableColumn id="10" name="Sent KB/sec" dataDxfId="1"/>
+    <tableColumn id="11" name="Avg. Bytes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3275,8 +3305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K54" sqref="K54"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3286,500 +3316,500 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B3" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>126201</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>126201</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>111213</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>111213</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>111132</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>111132</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>97838</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>97838</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>97838</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>97838</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>89958</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <v>89958</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>89958</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>89958</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>88205</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>88205</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>83514</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="3">
         <v>83514</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <v>83514</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="3">
         <v>83514</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="3">
         <v>67277</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="3">
         <v>67277</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>65377</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="3">
         <v>65377</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="3">
         <v>65377</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="3">
         <v>65377</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="3">
         <v>55120</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="3">
         <v>55120</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="3">
         <v>49068</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="3">
         <v>49068</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="3">
         <v>46138</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="3">
         <v>46138</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="3">
         <v>41757</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="3">
         <v>41757</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="3">
         <v>41340</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="3">
         <v>41340</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="3">
         <v>40710</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="3">
         <v>40710</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="3">
         <v>40410</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23" s="3">
         <v>40410</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="3">
         <v>39817</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F24" s="4">
+      <c r="F24" s="3">
         <v>39817</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="3">
         <v>39527</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F25" s="3">
         <v>39527</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="3">
         <v>37996</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F26" s="4">
+      <c r="F26" s="3">
         <v>37996</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="4">
-        <v>0</v>
-      </c>
-      <c r="E27" s="3" t="s">
+      <c r="B27" s="3">
+        <v>0</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F27" s="4">
-        <v>0</v>
+      <c r="F27" s="3">
+        <v>320</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="4">
-        <v>0</v>
-      </c>
-      <c r="E28" s="3" t="s">
+      <c r="B28" s="3">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F28" s="4">
-        <v>0</v>
+      <c r="F28" s="3">
+        <v>310</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="4">
-        <v>0</v>
-      </c>
-      <c r="E29" s="3" t="s">
+      <c r="B29" s="3">
+        <v>0</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F29" s="4">
-        <v>0</v>
+      <c r="F29" s="3">
+        <v>200</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="4">
-        <v>0</v>
-      </c>
-      <c r="E30" s="3" t="s">
+      <c r="B30" s="3">
+        <v>0</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F30" s="4">
-        <v>0</v>
+      <c r="F30" s="3">
+        <v>190</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="4">
-        <v>0</v>
-      </c>
-      <c r="E31" s="3" t="s">
+      <c r="B31" s="3">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F31" s="4">
-        <v>0</v>
+      <c r="F31" s="3">
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="4">
-        <v>0</v>
-      </c>
-      <c r="E32" s="3" t="s">
+      <c r="B32" s="3">
+        <v>0</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F32" s="4">
-        <v>0</v>
+      <c r="F32" s="3">
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="4">
-        <v>0</v>
-      </c>
-      <c r="E33" s="3" t="s">
+      <c r="B33" s="3">
+        <v>0</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F33" s="4">
-        <v>0</v>
+      <c r="F33" s="3">
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="4">
-        <v>0</v>
-      </c>
-      <c r="E34" s="3" t="s">
+      <c r="B34" s="3">
+        <v>0</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F34" s="4">
-        <v>0</v>
+      <c r="F34" s="3">
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B35" s="4">
-        <v>0</v>
-      </c>
-      <c r="E35" s="3" t="s">
+      <c r="B35" s="3">
+        <v>0</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F35" s="4">
-        <v>0</v>
+      <c r="F35" s="3">
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="4">
-        <v>0</v>
-      </c>
-      <c r="E36" s="3" t="s">
+      <c r="B36" s="3">
+        <v>0</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F36" s="4">
-        <v>0</v>
+      <c r="F36" s="3">
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B37" s="4">
-        <v>0</v>
-      </c>
-      <c r="E37" s="3" t="s">
+      <c r="B37" s="3">
+        <v>0</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F37" s="4">
-        <v>0</v>
+      <c r="F37" s="3">
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B38" s="3">
         <v>47331.911764705881</v>
       </c>
     </row>
@@ -3794,19 +3824,23 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:XFD36"/>
+      <selection activeCell="D15" sqref="A1:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -3814,1363 +3848,1363 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="5">
+        <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
+        <v>126201</v>
+      </c>
+      <c r="C2" s="5">
+        <v>1357</v>
+      </c>
+      <c r="D2" s="5">
+        <v>93</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5">
+        <v>536</v>
+      </c>
+      <c r="G2" s="5">
+        <v>51.84</v>
+      </c>
+      <c r="H2" s="5">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5">
+        <v>3.8162699999999998</v>
+      </c>
+      <c r="J2" s="5">
+        <v>44.1</v>
+      </c>
+      <c r="K2" s="5">
+        <v>15.31</v>
+      </c>
+      <c r="L2" s="5">
+        <v>11832</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="5">
+        <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
+        <v>111213</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1373</v>
+      </c>
+      <c r="D3" s="5">
+        <v>81</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5">
+        <v>425</v>
+      </c>
+      <c r="G3" s="5">
+        <v>43.36</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5">
+        <v>3.83663</v>
+      </c>
+      <c r="J3" s="5">
+        <v>43.39</v>
+      </c>
+      <c r="K3" s="5">
+        <v>10.08</v>
+      </c>
+      <c r="L3" s="5">
+        <v>11582</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="5">
+        <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
+        <v>111132</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1372</v>
+      </c>
+      <c r="D4" s="5">
+        <v>81</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>425</v>
+      </c>
+      <c r="G4" s="5">
+        <v>43.42</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5">
+        <v>3.8357899999999998</v>
+      </c>
+      <c r="J4" s="5">
+        <v>61.93</v>
+      </c>
+      <c r="K4" s="5">
+        <v>10.08</v>
+      </c>
+      <c r="L4" s="5">
+        <v>16533.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="5">
+        <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
+        <v>97838</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1378</v>
+      </c>
+      <c r="D5" s="5">
+        <v>71</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
+        <v>408</v>
+      </c>
+      <c r="G5" s="5">
+        <v>40.08</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="5">
+        <v>3.84165</v>
+      </c>
+      <c r="J5" s="5">
+        <v>27.26</v>
+      </c>
+      <c r="K5" s="5">
+        <v>9.9700000000000006</v>
+      </c>
+      <c r="L5" s="5">
+        <v>7266.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="5">
+        <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
+        <v>97838</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1378</v>
+      </c>
+      <c r="D6" s="5">
+        <v>71</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
+        <v>408</v>
+      </c>
+      <c r="G6" s="5">
+        <v>40.08</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5">
+        <v>3.84165</v>
+      </c>
+      <c r="J6" s="5">
+        <v>27.26</v>
+      </c>
+      <c r="K6" s="5">
+        <v>9.9700000000000006</v>
+      </c>
+      <c r="L6" s="5">
+        <v>7266.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="5">
+        <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
+        <v>89958</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1363</v>
+      </c>
+      <c r="D7" s="5">
+        <v>66</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0</v>
+      </c>
+      <c r="F7" s="5">
+        <v>508</v>
+      </c>
+      <c r="G7" s="5">
+        <v>39.51</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0</v>
+      </c>
+      <c r="I7" s="5">
+        <v>3.8208600000000001</v>
+      </c>
+      <c r="J7" s="5">
+        <v>26.48</v>
+      </c>
+      <c r="K7" s="5">
+        <v>10.62</v>
+      </c>
+      <c r="L7" s="5">
+        <v>7097.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="5">
+        <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
+        <v>89958</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1363</v>
+      </c>
+      <c r="D8" s="5">
+        <v>66</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5">
+        <v>508</v>
+      </c>
+      <c r="G8" s="5">
+        <v>39.51</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5">
+        <v>3.8208600000000001</v>
+      </c>
+      <c r="J8" s="5">
+        <v>26.48</v>
+      </c>
+      <c r="K8" s="5">
+        <v>10.62</v>
+      </c>
+      <c r="L8" s="5">
+        <v>7097.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="5">
+        <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
+        <v>88205</v>
+      </c>
+      <c r="C9" s="5">
+        <v>1357</v>
+      </c>
+      <c r="D9" s="5">
+        <v>65</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
+      <c r="F9" s="5">
+        <v>425</v>
+      </c>
+      <c r="G9" s="5">
+        <v>37.630000000000003</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5">
+        <v>3.8165800000000001</v>
+      </c>
+      <c r="J9" s="5">
+        <v>27.53</v>
+      </c>
+      <c r="K9" s="5">
+        <v>11.27</v>
+      </c>
+      <c r="L9" s="5">
+        <v>7386.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="5">
+        <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
+        <v>83514</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1347</v>
+      </c>
+      <c r="D10" s="5">
+        <v>62</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0</v>
+      </c>
+      <c r="F10" s="5">
+        <v>396</v>
+      </c>
+      <c r="G10" s="5">
+        <v>42.8</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5">
+        <v>3.8020999999999998</v>
+      </c>
+      <c r="J10" s="5">
+        <v>25.6</v>
+      </c>
+      <c r="K10" s="5">
+        <v>10.06</v>
+      </c>
+      <c r="L10" s="5">
+        <v>6893.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="5">
+        <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
+        <v>83514</v>
+      </c>
+      <c r="C11" s="5">
+        <v>1347</v>
+      </c>
+      <c r="D11" s="5">
+        <v>62</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5">
+        <v>396</v>
+      </c>
+      <c r="G11" s="5">
+        <v>42.8</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0</v>
+      </c>
+      <c r="I11" s="5">
+        <v>3.8020999999999998</v>
+      </c>
+      <c r="J11" s="5">
+        <v>25.6</v>
+      </c>
+      <c r="K11" s="5">
+        <v>10.06</v>
+      </c>
+      <c r="L11" s="5">
+        <v>6893.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="5">
+        <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
+        <v>67277</v>
+      </c>
+      <c r="C12" s="5">
+        <v>1373</v>
+      </c>
+      <c r="D12" s="5">
+        <v>49</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5">
+        <v>216</v>
+      </c>
+      <c r="G12" s="5">
+        <v>25.09</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0</v>
+      </c>
+      <c r="I12" s="5">
+        <v>3.8368600000000002</v>
+      </c>
+      <c r="J12" s="5">
+        <v>11.34</v>
+      </c>
+      <c r="K12" s="5">
+        <v>4.47</v>
+      </c>
+      <c r="L12" s="5">
+        <v>3026.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B2">
-        <v>1391</v>
-      </c>
-      <c r="C2">
-        <v>47</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>240</v>
-      </c>
-      <c r="F2">
-        <v>23.65</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>3.8640599999999998</v>
-      </c>
-      <c r="I2">
-        <v>37.29</v>
-      </c>
-      <c r="J2">
-        <v>1.78</v>
-      </c>
-      <c r="K2">
-        <v>9881.2000000000007</v>
-      </c>
-      <c r="L2">
+      <c r="B13" s="5">
         <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
         <v>65377</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3">
+      <c r="C13" s="5">
         <v>1391</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>0.5</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>3.8645100000000001</v>
-      </c>
-      <c r="I3">
-        <v>12.56</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>3326.8</v>
-      </c>
-      <c r="L3">
-        <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4">
-        <v>1391</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>8</v>
-      </c>
-      <c r="F4">
-        <v>0.52</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>3.8645100000000001</v>
-      </c>
-      <c r="I4">
-        <v>12.58</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>3333.8</v>
-      </c>
-      <c r="L4">
-        <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="D13" s="5">
+        <v>47</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0</v>
+      </c>
+      <c r="F13" s="5">
+        <v>240</v>
+      </c>
+      <c r="G13" s="5">
+        <v>23.65</v>
+      </c>
+      <c r="H13" s="5">
+        <v>0</v>
+      </c>
+      <c r="I13" s="5">
+        <v>3.8640599999999998</v>
+      </c>
+      <c r="J13" s="5">
+        <v>37.29</v>
+      </c>
+      <c r="K13" s="5">
+        <v>1.78</v>
+      </c>
+      <c r="L13" s="5">
+        <v>9881.2000000000007</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B5">
-        <v>1391</v>
-      </c>
-      <c r="C5">
-        <v>47</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>240</v>
-      </c>
-      <c r="F5">
-        <v>23.65</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>3.8640500000000002</v>
-      </c>
-      <c r="I5">
-        <v>37.29</v>
-      </c>
-      <c r="J5">
-        <v>1.78</v>
-      </c>
-      <c r="K5">
-        <v>9881.2000000000007</v>
-      </c>
-      <c r="L5">
+      <c r="B14" s="5">
         <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
         <v>65377</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6">
+      <c r="C14" s="5">
+        <v>1391</v>
+      </c>
+      <c r="D14" s="5">
+        <v>47</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0</v>
+      </c>
+      <c r="F14" s="5">
+        <v>240</v>
+      </c>
+      <c r="G14" s="5">
+        <v>23.65</v>
+      </c>
+      <c r="H14" s="5">
+        <v>0</v>
+      </c>
+      <c r="I14" s="5">
+        <v>3.8640500000000002</v>
+      </c>
+      <c r="J14" s="5">
+        <v>37.29</v>
+      </c>
+      <c r="K14" s="5">
+        <v>1.78</v>
+      </c>
+      <c r="L14" s="5">
+        <v>9881.2000000000007</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="5">
+        <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
+        <v>55120</v>
+      </c>
+      <c r="C15" s="5">
         <v>1378</v>
       </c>
-      <c r="C6">
-        <v>71</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>408</v>
-      </c>
-      <c r="F6">
-        <v>40.08</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>3.84165</v>
-      </c>
-      <c r="I6">
-        <v>27.26</v>
-      </c>
-      <c r="J6">
-        <v>9.9700000000000006</v>
-      </c>
-      <c r="K6">
-        <v>7266.7</v>
-      </c>
-      <c r="L6">
+      <c r="D15" s="5">
+        <v>40</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0</v>
+      </c>
+      <c r="F15" s="5">
+        <v>236</v>
+      </c>
+      <c r="G15" s="5">
+        <v>22.13</v>
+      </c>
+      <c r="H15" s="5">
+        <v>0</v>
+      </c>
+      <c r="I15" s="5">
+        <v>3.84185</v>
+      </c>
+      <c r="J15" s="5">
+        <v>9.07</v>
+      </c>
+      <c r="K15" s="5">
+        <v>4.45</v>
+      </c>
+      <c r="L15" s="5">
+        <v>2418.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="5">
         <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
-        <v>97838</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+        <v>49068</v>
+      </c>
+      <c r="C16" s="5">
+        <v>1363</v>
+      </c>
+      <c r="D16" s="5">
+        <v>36</v>
+      </c>
+      <c r="E16" s="5">
+        <v>0</v>
+      </c>
+      <c r="F16" s="5">
+        <v>184</v>
+      </c>
+      <c r="G16" s="5">
+        <v>20.74</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0</v>
+      </c>
+      <c r="I16" s="5">
+        <v>3.8210799999999998</v>
+      </c>
+      <c r="J16" s="5">
+        <v>7.63</v>
+      </c>
+      <c r="K16" s="5">
+        <v>4.45</v>
+      </c>
+      <c r="L16" s="5">
+        <v>2045.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="5">
+        <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
+        <v>46138</v>
+      </c>
+      <c r="C17" s="5">
+        <v>1357</v>
+      </c>
+      <c r="D17" s="5">
+        <v>34</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0</v>
+      </c>
+      <c r="F17" s="5">
+        <v>200</v>
+      </c>
+      <c r="G17" s="5">
+        <v>19.64</v>
+      </c>
+      <c r="H17" s="5">
+        <v>0</v>
+      </c>
+      <c r="I17" s="5">
+        <v>3.81677</v>
+      </c>
+      <c r="J17" s="5">
+        <v>8.0299999999999994</v>
+      </c>
+      <c r="K17" s="5">
+        <v>4.45</v>
+      </c>
+      <c r="L17" s="5">
+        <v>2154.8000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="5">
+        <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
+        <v>41757</v>
+      </c>
+      <c r="C18" s="5">
+        <v>1347</v>
+      </c>
+      <c r="D18" s="5">
+        <v>31</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0</v>
+      </c>
+      <c r="F18" s="5">
+        <v>244</v>
+      </c>
+      <c r="G18" s="5">
+        <v>25.31</v>
+      </c>
+      <c r="H18" s="5">
+        <v>0</v>
+      </c>
+      <c r="I18" s="5">
+        <v>3.8023400000000001</v>
+      </c>
+      <c r="J18" s="5">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="K18" s="5">
+        <v>5.63</v>
+      </c>
+      <c r="L18" s="5">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>16</v>
       </c>
-      <c r="B7">
-        <v>1378</v>
-      </c>
-      <c r="C7">
-        <v>30</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>275</v>
-      </c>
-      <c r="F7">
-        <v>21.7</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>3.8420000000000001</v>
-      </c>
-      <c r="I7">
-        <v>4.45</v>
-      </c>
-      <c r="J7">
-        <v>5.52</v>
-      </c>
-      <c r="K7">
-        <v>1187</v>
-      </c>
-      <c r="L7">
+      <c r="B19" s="5">
         <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
         <v>41340</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8">
+      <c r="C19" s="5">
         <v>1378</v>
       </c>
-      <c r="C8">
-        <v>40</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>236</v>
-      </c>
-      <c r="F8">
-        <v>22.13</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>3.84185</v>
-      </c>
-      <c r="I8">
-        <v>9.07</v>
-      </c>
-      <c r="J8">
+      <c r="D19" s="5">
+        <v>30</v>
+      </c>
+      <c r="E19" s="5">
+        <v>0</v>
+      </c>
+      <c r="F19" s="5">
+        <v>275</v>
+      </c>
+      <c r="G19" s="5">
+        <v>21.7</v>
+      </c>
+      <c r="H19" s="5">
+        <v>0</v>
+      </c>
+      <c r="I19" s="5">
+        <v>3.8420000000000001</v>
+      </c>
+      <c r="J19" s="5">
         <v>4.45</v>
       </c>
-      <c r="K8">
-        <v>2418.6</v>
-      </c>
-      <c r="L8">
+      <c r="K19" s="5">
+        <v>5.52</v>
+      </c>
+      <c r="L19" s="5">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="5">
         <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
-        <v>55120</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9">
-        <v>1378</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-      <c r="F9">
-        <v>0.5</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>3.8422900000000002</v>
-      </c>
-      <c r="I9">
-        <v>13.74</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>3661.1</v>
-      </c>
-      <c r="L9">
+        <v>40710</v>
+      </c>
+      <c r="C20" s="5">
+        <v>1357</v>
+      </c>
+      <c r="D20" s="5">
+        <v>30</v>
+      </c>
+      <c r="E20" s="5">
+        <v>0</v>
+      </c>
+      <c r="F20" s="5">
+        <v>266</v>
+      </c>
+      <c r="G20" s="5">
+        <v>20.74</v>
+      </c>
+      <c r="H20" s="5">
+        <v>0</v>
+      </c>
+      <c r="I20" s="5">
+        <v>3.8168700000000002</v>
+      </c>
+      <c r="J20" s="5">
+        <v>4.42</v>
+      </c>
+      <c r="K20" s="5">
+        <v>6.82</v>
+      </c>
+      <c r="L20" s="5">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="5">
         <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10">
-        <v>1378</v>
-      </c>
-      <c r="C10">
-        <v>71</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>408</v>
-      </c>
-      <c r="F10">
-        <v>40.08</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>3.84165</v>
-      </c>
-      <c r="I10">
-        <v>27.26</v>
-      </c>
-      <c r="J10">
-        <v>9.9700000000000006</v>
-      </c>
-      <c r="K10">
-        <v>7266.7</v>
-      </c>
-      <c r="L10">
-        <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
-        <v>97838</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11">
-        <v>1373</v>
-      </c>
-      <c r="C11">
-        <v>81</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>425</v>
-      </c>
-      <c r="F11">
-        <v>43.36</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>3.83663</v>
-      </c>
-      <c r="I11">
-        <v>43.39</v>
-      </c>
-      <c r="J11">
-        <v>10.08</v>
-      </c>
-      <c r="K11">
-        <v>11582</v>
-      </c>
-      <c r="L11">
-        <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
-        <v>111213</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+        <v>40410</v>
+      </c>
+      <c r="C21" s="5">
+        <v>1347</v>
+      </c>
+      <c r="D21" s="5">
+        <v>30</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0</v>
+      </c>
+      <c r="F21" s="5">
+        <v>200</v>
+      </c>
+      <c r="G21" s="5">
+        <v>19.95</v>
+      </c>
+      <c r="H21" s="5">
+        <v>0</v>
+      </c>
+      <c r="I21" s="5">
+        <v>3.8022900000000002</v>
+      </c>
+      <c r="J21" s="5">
+        <v>7.27</v>
+      </c>
+      <c r="K21" s="5">
+        <v>4.42</v>
+      </c>
+      <c r="L21" s="5">
+        <v>1959</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="B12">
-        <v>1373</v>
-      </c>
-      <c r="C12">
-        <v>29</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>250</v>
-      </c>
-      <c r="F12">
-        <v>21.46</v>
-      </c>
-      <c r="G12" s="1">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>3.8370899999999999</v>
-      </c>
-      <c r="I12">
-        <v>4.45</v>
-      </c>
-      <c r="J12">
-        <v>5.62</v>
-      </c>
-      <c r="K12">
-        <v>1187</v>
-      </c>
-      <c r="L12">
+      <c r="B22" s="5">
         <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
         <v>39817</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13">
+      <c r="C22" s="5">
         <v>1373</v>
       </c>
-      <c r="C13">
-        <v>49</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>216</v>
-      </c>
-      <c r="F13">
-        <v>25.09</v>
-      </c>
-      <c r="G13" s="1">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>3.8368600000000002</v>
-      </c>
-      <c r="I13">
-        <v>11.34</v>
-      </c>
-      <c r="J13">
-        <v>4.47</v>
-      </c>
-      <c r="K13">
-        <v>3026.4</v>
-      </c>
-      <c r="L13">
-        <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
-        <v>67277</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14">
-        <v>1373</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>2</v>
-      </c>
-      <c r="F14">
-        <v>0.5</v>
-      </c>
-      <c r="G14" s="1">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>3.83717</v>
-      </c>
-      <c r="I14">
-        <v>13.74</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>3666.5</v>
-      </c>
-      <c r="L14">
-        <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15">
-        <v>1373</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>7</v>
-      </c>
-      <c r="F15">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="G15" s="1">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>3.8374299999999999</v>
-      </c>
-      <c r="I15">
-        <v>13.87</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>3702.2</v>
-      </c>
-      <c r="L15">
-        <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16">
-        <v>1372</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>3</v>
-      </c>
-      <c r="F16">
-        <v>0.52</v>
-      </c>
-      <c r="G16" s="1">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>3.83657</v>
-      </c>
-      <c r="I16">
-        <v>18.55</v>
-      </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <v>4951.3</v>
-      </c>
-      <c r="L16">
-        <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17">
-        <v>1372</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17">
-        <v>0.44</v>
-      </c>
-      <c r="G17" s="1">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>3.83657</v>
-      </c>
-      <c r="I17">
-        <v>9.83</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="K17">
-        <v>2624.1</v>
-      </c>
-      <c r="L17">
-        <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18">
-        <v>1372</v>
-      </c>
-      <c r="C18">
-        <v>81</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>425</v>
-      </c>
-      <c r="F18">
-        <v>43.42</v>
-      </c>
-      <c r="G18" s="1">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>3.8357899999999998</v>
-      </c>
-      <c r="I18">
-        <v>61.93</v>
-      </c>
-      <c r="J18">
-        <v>10.08</v>
-      </c>
-      <c r="K18">
-        <v>16533.2</v>
-      </c>
-      <c r="L18">
-        <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
-        <v>111132</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19">
-        <v>1363</v>
-      </c>
-      <c r="C19">
-        <v>66</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>508</v>
-      </c>
-      <c r="F19">
-        <v>39.51</v>
-      </c>
-      <c r="G19" s="1">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>3.8208600000000001</v>
-      </c>
-      <c r="I19">
-        <v>26.48</v>
-      </c>
-      <c r="J19">
-        <v>10.62</v>
-      </c>
-      <c r="K19">
-        <v>7097.2</v>
-      </c>
-      <c r="L19">
-        <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
-        <v>89958</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="D22" s="5">
         <v>29</v>
       </c>
-      <c r="B20">
-        <v>1363</v>
-      </c>
-      <c r="C20">
+      <c r="E22" s="5">
+        <v>0</v>
+      </c>
+      <c r="F22" s="5">
+        <v>250</v>
+      </c>
+      <c r="G22" s="5">
+        <v>21.46</v>
+      </c>
+      <c r="H22" s="5">
+        <v>0</v>
+      </c>
+      <c r="I22" s="5">
+        <v>3.8370899999999999</v>
+      </c>
+      <c r="J22" s="5">
+        <v>4.45</v>
+      </c>
+      <c r="K22" s="5">
+        <v>5.62</v>
+      </c>
+      <c r="L22" s="5">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>29</v>
       </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>335</v>
-      </c>
-      <c r="F20">
-        <v>21.85</v>
-      </c>
-      <c r="G20" s="1">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>3.8212100000000002</v>
-      </c>
-      <c r="I20">
-        <v>4.43</v>
-      </c>
-      <c r="J20">
-        <v>6.17</v>
-      </c>
-      <c r="K20">
-        <v>1187</v>
-      </c>
-      <c r="L20">
+      <c r="B23" s="5">
         <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
         <v>39527</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21">
+      <c r="C23" s="5">
         <v>1363</v>
       </c>
-      <c r="C21">
-        <v>36</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>184</v>
-      </c>
-      <c r="F21">
-        <v>20.74</v>
-      </c>
-      <c r="G21" s="1">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>3.8210799999999998</v>
-      </c>
-      <c r="I21">
-        <v>7.63</v>
-      </c>
-      <c r="J21">
-        <v>4.45</v>
-      </c>
-      <c r="K21">
-        <v>2045.4</v>
-      </c>
-      <c r="L21">
-        <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
-        <v>49068</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22">
-        <v>1363</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>3</v>
-      </c>
-      <c r="F22">
-        <v>0.52</v>
-      </c>
-      <c r="G22" s="1">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>3.8214299999999999</v>
-      </c>
-      <c r="I22">
-        <v>14.42</v>
-      </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
-      <c r="K22">
-        <v>3864.8</v>
-      </c>
-      <c r="L22">
-        <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23">
-        <v>1363</v>
-      </c>
-      <c r="C23">
-        <v>66</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>508</v>
-      </c>
-      <c r="F23">
-        <v>39.51</v>
-      </c>
-      <c r="G23" s="1">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>3.8208600000000001</v>
-      </c>
-      <c r="I23">
-        <v>26.48</v>
-      </c>
-      <c r="J23">
-        <v>10.62</v>
-      </c>
-      <c r="K23">
-        <v>7097.2</v>
-      </c>
-      <c r="L23">
-        <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
-        <v>89958</v>
+      <c r="D23" s="5">
+        <v>29</v>
+      </c>
+      <c r="E23" s="5">
+        <v>0</v>
+      </c>
+      <c r="F23" s="5">
+        <v>335</v>
+      </c>
+      <c r="G23" s="5">
+        <v>21.85</v>
+      </c>
+      <c r="H23" s="5">
+        <v>0</v>
+      </c>
+      <c r="I23" s="5">
+        <v>3.8212100000000002</v>
+      </c>
+      <c r="J23" s="5">
+        <v>4.43</v>
+      </c>
+      <c r="K23" s="5">
+        <v>6.17</v>
+      </c>
+      <c r="L23" s="5">
+        <v>1187</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24">
+        <v>37</v>
+      </c>
+      <c r="B24" s="5">
+        <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
+        <v>37996</v>
+      </c>
+      <c r="C24" s="5">
         <v>1357</v>
       </c>
-      <c r="C24">
-        <v>65</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>425</v>
-      </c>
-      <c r="F24">
-        <v>37.630000000000003</v>
-      </c>
-      <c r="G24" s="1">
-        <v>0</v>
-      </c>
-      <c r="H24">
-        <v>3.8165800000000001</v>
-      </c>
-      <c r="I24">
-        <v>27.53</v>
-      </c>
-      <c r="J24">
-        <v>11.27</v>
-      </c>
-      <c r="K24">
-        <v>7386.2</v>
-      </c>
-      <c r="L24">
-        <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
-        <v>88205</v>
+      <c r="D24" s="5">
+        <v>28</v>
+      </c>
+      <c r="E24" s="5">
+        <v>0</v>
+      </c>
+      <c r="F24" s="5">
+        <v>168</v>
+      </c>
+      <c r="G24" s="5">
+        <v>17.45</v>
+      </c>
+      <c r="H24" s="5">
+        <v>0</v>
+      </c>
+      <c r="I24" s="5">
+        <v>3.81684</v>
+      </c>
+      <c r="J24" s="5">
+        <v>16.57</v>
+      </c>
+      <c r="K24" s="5">
+        <v>4.05</v>
+      </c>
+      <c r="L24" s="5">
+        <v>4445.8</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25">
-        <v>1357</v>
-      </c>
-      <c r="C25">
-        <v>30</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>266</v>
-      </c>
-      <c r="F25">
-        <v>20.74</v>
-      </c>
-      <c r="G25" s="1">
-        <v>0</v>
-      </c>
-      <c r="H25">
-        <v>3.8168700000000002</v>
-      </c>
-      <c r="I25">
-        <v>4.42</v>
-      </c>
-      <c r="J25">
-        <v>6.82</v>
-      </c>
-      <c r="K25">
-        <v>1187</v>
-      </c>
-      <c r="L25">
+        <v>12</v>
+      </c>
+      <c r="B25" s="5">
         <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
-        <v>40710</v>
+        <v>0</v>
+      </c>
+      <c r="C25" s="5">
+        <v>1391</v>
+      </c>
+      <c r="D25" s="5">
+        <v>0</v>
+      </c>
+      <c r="E25" s="5">
+        <v>0</v>
+      </c>
+      <c r="F25" s="5">
+        <v>2</v>
+      </c>
+      <c r="G25" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="H25" s="5">
+        <v>0</v>
+      </c>
+      <c r="I25" s="5">
+        <v>3.8645100000000001</v>
+      </c>
+      <c r="J25" s="5">
+        <v>12.56</v>
+      </c>
+      <c r="K25" s="5">
+        <v>0</v>
+      </c>
+      <c r="L25" s="5">
+        <v>3326.8</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26">
-        <v>1357</v>
-      </c>
-      <c r="C26">
-        <v>34</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>200</v>
-      </c>
-      <c r="F26">
-        <v>19.64</v>
-      </c>
-      <c r="G26" s="1">
-        <v>0</v>
-      </c>
-      <c r="H26">
-        <v>3.81677</v>
-      </c>
-      <c r="I26">
-        <v>8.0299999999999994</v>
-      </c>
-      <c r="J26">
-        <v>4.45</v>
-      </c>
-      <c r="K26">
-        <v>2154.8000000000002</v>
-      </c>
-      <c r="L26">
+        <v>13</v>
+      </c>
+      <c r="B26" s="5">
         <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
-        <v>46138</v>
+        <v>0</v>
+      </c>
+      <c r="C26" s="5">
+        <v>1391</v>
+      </c>
+      <c r="D26" s="5">
+        <v>0</v>
+      </c>
+      <c r="E26" s="5">
+        <v>0</v>
+      </c>
+      <c r="F26" s="5">
+        <v>8</v>
+      </c>
+      <c r="G26" s="5">
+        <v>0.52</v>
+      </c>
+      <c r="H26" s="5">
+        <v>0</v>
+      </c>
+      <c r="I26" s="5">
+        <v>3.8645100000000001</v>
+      </c>
+      <c r="J26" s="5">
+        <v>12.58</v>
+      </c>
+      <c r="K26" s="5">
+        <v>0</v>
+      </c>
+      <c r="L26" s="5">
+        <v>3333.8</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27">
-        <v>1357</v>
-      </c>
-      <c r="C27">
-        <v>0</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>6</v>
-      </c>
-      <c r="F27">
-        <v>0.53</v>
-      </c>
-      <c r="G27" s="1">
-        <v>0</v>
-      </c>
-      <c r="H27">
-        <v>3.8170299999999999</v>
-      </c>
-      <c r="I27">
-        <v>15.08</v>
-      </c>
-      <c r="J27">
-        <v>0</v>
-      </c>
-      <c r="K27">
-        <v>4044.4</v>
-      </c>
-      <c r="L27">
+        <v>18</v>
+      </c>
+      <c r="B27" s="5">
         <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
         <v>0</v>
+      </c>
+      <c r="C27" s="5">
+        <v>1378</v>
+      </c>
+      <c r="D27" s="5">
+        <v>0</v>
+      </c>
+      <c r="E27" s="5">
+        <v>0</v>
+      </c>
+      <c r="F27" s="5">
+        <v>2</v>
+      </c>
+      <c r="G27" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="H27" s="5">
+        <v>0</v>
+      </c>
+      <c r="I27" s="5">
+        <v>3.8422900000000002</v>
+      </c>
+      <c r="J27" s="5">
+        <v>13.74</v>
+      </c>
+      <c r="K27" s="5">
+        <v>0</v>
+      </c>
+      <c r="L27" s="5">
+        <v>3661.1</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28">
-        <v>1357</v>
-      </c>
-      <c r="C28">
-        <v>28</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>168</v>
-      </c>
-      <c r="F28">
-        <v>17.45</v>
-      </c>
-      <c r="G28" s="1">
-        <v>0</v>
-      </c>
-      <c r="H28">
-        <v>3.81684</v>
-      </c>
-      <c r="I28">
-        <v>16.57</v>
-      </c>
-      <c r="J28">
-        <v>4.05</v>
-      </c>
-      <c r="K28">
-        <v>4445.8</v>
-      </c>
-      <c r="L28">
+        <v>23</v>
+      </c>
+      <c r="B28" s="5">
         <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
-        <v>37996</v>
+        <v>0</v>
+      </c>
+      <c r="C28" s="5">
+        <v>1373</v>
+      </c>
+      <c r="D28" s="5">
+        <v>0</v>
+      </c>
+      <c r="E28" s="5">
+        <v>0</v>
+      </c>
+      <c r="F28" s="5">
+        <v>2</v>
+      </c>
+      <c r="G28" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="H28" s="5">
+        <v>0</v>
+      </c>
+      <c r="I28" s="5">
+        <v>3.83717</v>
+      </c>
+      <c r="J28" s="5">
+        <v>13.74</v>
+      </c>
+      <c r="K28" s="5">
+        <v>0</v>
+      </c>
+      <c r="L28" s="5">
+        <v>3666.5</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29">
-        <v>1357</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>2</v>
-      </c>
-      <c r="F29">
-        <v>0.5</v>
-      </c>
-      <c r="G29" s="1">
-        <v>0</v>
-      </c>
-      <c r="H29">
-        <v>3.8172199999999998</v>
-      </c>
-      <c r="I29">
-        <v>12.55</v>
-      </c>
-      <c r="J29">
-        <v>0</v>
-      </c>
-      <c r="K29">
-        <v>3367.8</v>
-      </c>
-      <c r="L29">
+        <v>24</v>
+      </c>
+      <c r="B29" s="5">
         <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
         <v>0</v>
+      </c>
+      <c r="C29" s="5">
+        <v>1373</v>
+      </c>
+      <c r="D29" s="5">
+        <v>0</v>
+      </c>
+      <c r="E29" s="5">
+        <v>0</v>
+      </c>
+      <c r="F29" s="5">
+        <v>7</v>
+      </c>
+      <c r="G29" s="5">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H29" s="5">
+        <v>0</v>
+      </c>
+      <c r="I29" s="5">
+        <v>3.8374299999999999</v>
+      </c>
+      <c r="J29" s="5">
+        <v>13.87</v>
+      </c>
+      <c r="K29" s="5">
+        <v>0</v>
+      </c>
+      <c r="L29" s="5">
+        <v>3702.2</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>39</v>
-      </c>
-      <c r="B30">
-        <v>1357</v>
-      </c>
-      <c r="C30">
-        <v>93</v>
-      </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <v>536</v>
-      </c>
-      <c r="F30">
-        <v>51.84</v>
-      </c>
-      <c r="G30" s="1">
-        <v>0</v>
-      </c>
-      <c r="H30">
-        <v>3.8162699999999998</v>
-      </c>
-      <c r="I30">
-        <v>44.1</v>
-      </c>
-      <c r="J30">
-        <v>15.31</v>
-      </c>
-      <c r="K30">
-        <v>11832</v>
-      </c>
-      <c r="L30">
+        <v>25</v>
+      </c>
+      <c r="B30" s="5">
         <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
-        <v>126201</v>
+        <v>0</v>
+      </c>
+      <c r="C30" s="5">
+        <v>1372</v>
+      </c>
+      <c r="D30" s="5">
+        <v>0</v>
+      </c>
+      <c r="E30" s="5">
+        <v>0</v>
+      </c>
+      <c r="F30" s="5">
+        <v>3</v>
+      </c>
+      <c r="G30" s="5">
+        <v>0.52</v>
+      </c>
+      <c r="H30" s="5">
+        <v>0</v>
+      </c>
+      <c r="I30" s="5">
+        <v>3.83657</v>
+      </c>
+      <c r="J30" s="5">
+        <v>18.55</v>
+      </c>
+      <c r="K30" s="5">
+        <v>0</v>
+      </c>
+      <c r="L30" s="5">
+        <v>4951.3</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>40</v>
-      </c>
-      <c r="B31">
-        <v>1347</v>
-      </c>
-      <c r="C31">
-        <v>62</v>
-      </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>396</v>
-      </c>
-      <c r="F31">
-        <v>42.8</v>
-      </c>
-      <c r="G31" s="1">
-        <v>0</v>
-      </c>
-      <c r="H31">
-        <v>3.8020999999999998</v>
-      </c>
-      <c r="I31">
-        <v>25.6</v>
-      </c>
-      <c r="J31">
-        <v>10.06</v>
-      </c>
-      <c r="K31">
-        <v>6893.6</v>
-      </c>
-      <c r="L31">
+        <v>26</v>
+      </c>
+      <c r="B31" s="5">
         <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
-        <v>83514</v>
+        <v>0</v>
+      </c>
+      <c r="C31" s="5">
+        <v>1372</v>
+      </c>
+      <c r="D31" s="5">
+        <v>0</v>
+      </c>
+      <c r="E31" s="5">
+        <v>0</v>
+      </c>
+      <c r="F31" s="5">
+        <v>1</v>
+      </c>
+      <c r="G31" s="5">
+        <v>0.44</v>
+      </c>
+      <c r="H31" s="5">
+        <v>0</v>
+      </c>
+      <c r="I31" s="5">
+        <v>3.83657</v>
+      </c>
+      <c r="J31" s="5">
+        <v>9.83</v>
+      </c>
+      <c r="K31" s="5">
+        <v>0</v>
+      </c>
+      <c r="L31" s="5">
+        <v>2624.1</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>41</v>
-      </c>
-      <c r="B32">
-        <v>1347</v>
-      </c>
-      <c r="C32">
         <v>31</v>
       </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32">
-        <v>244</v>
-      </c>
-      <c r="F32">
-        <v>25.31</v>
-      </c>
-      <c r="G32" s="1">
-        <v>0</v>
-      </c>
-      <c r="H32">
-        <v>3.8023400000000001</v>
-      </c>
-      <c r="I32">
-        <v>4.3899999999999997</v>
-      </c>
-      <c r="J32">
-        <v>5.63</v>
-      </c>
-      <c r="K32">
-        <v>1183</v>
-      </c>
-      <c r="L32">
+      <c r="B32" s="5">
         <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
-        <v>41757</v>
+        <v>0</v>
+      </c>
+      <c r="C32" s="5">
+        <v>1363</v>
+      </c>
+      <c r="D32" s="5">
+        <v>0</v>
+      </c>
+      <c r="E32" s="5">
+        <v>0</v>
+      </c>
+      <c r="F32" s="5">
+        <v>3</v>
+      </c>
+      <c r="G32" s="5">
+        <v>0.52</v>
+      </c>
+      <c r="H32" s="5">
+        <v>0</v>
+      </c>
+      <c r="I32" s="5">
+        <v>3.8214299999999999</v>
+      </c>
+      <c r="J32" s="5">
+        <v>14.42</v>
+      </c>
+      <c r="K32" s="5">
+        <v>0</v>
+      </c>
+      <c r="L32" s="5">
+        <v>3864.8</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>42</v>
-      </c>
-      <c r="B33">
-        <v>1347</v>
-      </c>
-      <c r="C33">
-        <v>30</v>
-      </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33">
-        <v>200</v>
-      </c>
-      <c r="F33">
-        <v>19.95</v>
-      </c>
-      <c r="G33" s="1">
-        <v>0</v>
-      </c>
-      <c r="H33">
-        <v>3.8022900000000002</v>
-      </c>
-      <c r="I33">
-        <v>7.27</v>
-      </c>
-      <c r="J33">
-        <v>4.42</v>
-      </c>
-      <c r="K33">
-        <v>1959</v>
-      </c>
-      <c r="L33">
+        <v>36</v>
+      </c>
+      <c r="B33" s="5">
         <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
-        <v>40410</v>
+        <v>0</v>
+      </c>
+      <c r="C33" s="5">
+        <v>1357</v>
+      </c>
+      <c r="D33" s="5">
+        <v>0</v>
+      </c>
+      <c r="E33" s="5">
+        <v>0</v>
+      </c>
+      <c r="F33" s="5">
+        <v>6</v>
+      </c>
+      <c r="G33" s="5">
+        <v>0.53</v>
+      </c>
+      <c r="H33" s="5">
+        <v>0</v>
+      </c>
+      <c r="I33" s="5">
+        <v>3.8170299999999999</v>
+      </c>
+      <c r="J33" s="5">
+        <v>15.08</v>
+      </c>
+      <c r="K33" s="5">
+        <v>0</v>
+      </c>
+      <c r="L33" s="5">
+        <v>4044.4</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>43</v>
-      </c>
-      <c r="B34">
-        <v>1347</v>
-      </c>
-      <c r="C34">
-        <v>0</v>
-      </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-      <c r="E34">
-        <v>8</v>
-      </c>
-      <c r="F34">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="G34" s="1">
-        <v>0</v>
-      </c>
-      <c r="H34">
-        <v>3.8025899999999999</v>
-      </c>
-      <c r="I34">
-        <v>13.93</v>
-      </c>
-      <c r="J34">
-        <v>0</v>
-      </c>
-      <c r="K34">
-        <v>3751.6</v>
-      </c>
-      <c r="L34">
+        <v>38</v>
+      </c>
+      <c r="B34" s="5">
         <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
         <v>0</v>
+      </c>
+      <c r="C34" s="5">
+        <v>1357</v>
+      </c>
+      <c r="D34" s="5">
+        <v>0</v>
+      </c>
+      <c r="E34" s="5">
+        <v>0</v>
+      </c>
+      <c r="F34" s="5">
+        <v>2</v>
+      </c>
+      <c r="G34" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="H34" s="5">
+        <v>0</v>
+      </c>
+      <c r="I34" s="5">
+        <v>3.8172199999999998</v>
+      </c>
+      <c r="J34" s="5">
+        <v>12.55</v>
+      </c>
+      <c r="K34" s="5">
+        <v>0</v>
+      </c>
+      <c r="L34" s="5">
+        <v>3367.8</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>44</v>
-      </c>
-      <c r="B35">
+        <v>43</v>
+      </c>
+      <c r="B35" s="5">
+        <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
+        <v>0</v>
+      </c>
+      <c r="C35" s="5">
         <v>1347</v>
       </c>
-      <c r="C35">
-        <v>62</v>
-      </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="E35">
-        <v>396</v>
-      </c>
-      <c r="F35">
-        <v>42.8</v>
-      </c>
-      <c r="G35" s="1">
-        <v>0</v>
-      </c>
-      <c r="H35">
-        <v>3.8020999999999998</v>
-      </c>
-      <c r="I35">
-        <v>25.6</v>
-      </c>
-      <c r="J35">
-        <v>10.06</v>
-      </c>
-      <c r="K35">
-        <v>6893.6</v>
-      </c>
-      <c r="L35">
-        <f>Table1[[#This Row],['# Samples]]*Table1[[#This Row],[Average]]</f>
-        <v>83514</v>
+      <c r="D35" s="5">
+        <v>0</v>
+      </c>
+      <c r="E35" s="5">
+        <v>0</v>
+      </c>
+      <c r="F35" s="5">
+        <v>8</v>
+      </c>
+      <c r="G35" s="5">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H35" s="5">
+        <v>0</v>
+      </c>
+      <c r="I35" s="5">
+        <v>3.8025899999999999</v>
+      </c>
+      <c r="J35" s="5">
+        <v>13.93</v>
+      </c>
+      <c r="K35" s="5">
+        <v>0</v>
+      </c>
+      <c r="L35" s="5">
+        <v>3751.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>